<commit_message>
Update disclaimer on template
</commit_message>
<xml_diff>
--- a/docs/output_template.xlsx
+++ b/docs/output_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keith.Ng\Code\review-of-social-housing\outputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mhud-my.sharepoint.com/personal/keith_ng_hud_govt_nz/Documents/Code/hud-idi/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBAF8967-F15D-49FA-AFDA-F9BECC0DEFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{BBAF8967-F15D-49FA-AFDA-F9BECC0DEFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35C4D5C7-8123-4AD7-A2DB-6543D986F737}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22680" windowHeight="15192" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22680" windowHeight="15192" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Disclaimer" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,8 @@
     <t>Disclaimer</t>
   </si>
   <si>
-    <t>These results are not official statistics. They have been created for research purposes from the Integrated Data Infrastructure (IDI), managed by Stats NZ. For more information about the IDI, please visit https://www.stats.govt.nz/integrated-data/.
+    <t>Access to the data used in this study was provided by Stats NZ under conditions designed to give effect to the security and confidentiality provisions of the Data and Statistics Act 2022. The results presented in this study are the work of the author, not Stats NZ or individual data suppliers. 
+These results are not official statistics. They have been created for research purposes from the Integrated Data Infrastructure (IDI), managed by Stats NZ. For more information about the IDI, please visit https://www.stats.govt.nz/integrated-data/.
 The results are based in part on tax data supplied by Inland Revenue to Stats NZ under the Tax Administration Act 1994 for statistical purposes. Any discussion of data limirations or weaknesses is in the context of using the IDI for statistical purposes, and is not related to the data's ability to support Inland Revenue's core operational requirements.</t>
   </si>
 </sst>
@@ -445,7 +446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:K20"/>
     </sheetView>
   </sheetViews>
@@ -557,7 +558,7 @@
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="4" t="s">
         <v>1</v>
@@ -1329,7 +1330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AL1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>

</xml_diff>